<commit_message>
add row module tracuuluongthue
</commit_message>
<xml_diff>
--- a/app/webroot/phpexcel/mau/mau_phucaptienluong.xlsx
+++ b/app/webroot/phpexcel/mau/mau_phucaptienluong.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpxq2/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/eoffice/app/webroot/phpexcel/mau/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282753D2-20D3-6640-90FB-521256B909FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8D8239-71EC-0A4B-85F1-13B064A9A046}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="4560" windowWidth="25640" windowHeight="14440" xr2:uid="{D3715A52-7257-8646-8FEA-9AD953CFEB67}"/>
+    <workbookView xWindow="4300" yWindow="4960" windowWidth="25640" windowHeight="14440" xr2:uid="{D3715A52-7257-8646-8FEA-9AD953CFEB67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>BẢNG THANH TOÁN LƯƠNG VÀ PHỤ CẤP</t>
   </si>
@@ -111,10 +111,19 @@
     <t>C</t>
   </si>
   <si>
-    <t>NGUYỄN VĂN A</t>
-  </si>
-  <si>
-    <t>NGÔ VĂN B</t>
+    <t>PHẠM MINH TUẤN</t>
+  </si>
+  <si>
+    <t>NGUYỄN ĐĂNG KHANH</t>
+  </si>
+  <si>
+    <t>NGUYỄN SONG LY</t>
+  </si>
+  <si>
+    <t>NINH VĂN ANH</t>
+  </si>
+  <si>
+    <t>Quản lý phí</t>
   </si>
 </sst>
 </file>
@@ -302,75 +311,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,414 +698,605 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3EEB91E-2670-3B49-84E1-627490224321}">
-  <dimension ref="A2:AC8"/>
+  <dimension ref="A2:AE10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection sqref="A1:AC8"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="136" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="I2" s="1" t="s">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="I2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="15"/>
+      <c r="E4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3" t="s">
+      <c r="F4" s="15"/>
+      <c r="G4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3" t="s">
+      <c r="H4" s="15"/>
+      <c r="I4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3" t="s">
+      <c r="J4" s="15"/>
+      <c r="K4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3" t="s">
+      <c r="L4" s="15"/>
+      <c r="M4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3" t="s">
+      <c r="N4" s="15"/>
+      <c r="O4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3" t="s">
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3" t="s">
+      <c r="R4" s="15"/>
+      <c r="S4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="V4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3" t="s">
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+      <c r="Z4" s="15"/>
+      <c r="AA4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="AB4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AA4" s="4" t="s">
+      <c r="AC4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AD4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AE4" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="5" t="s">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="Q5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="R5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="S5" s="3"/>
-      <c r="T5" s="5" t="s">
+      <c r="S5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5" s="15"/>
+      <c r="V5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="W5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="V5" s="5" t="s">
+      <c r="X5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="W5" s="5" t="s">
+      <c r="Y5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="X5" s="5" t="s">
+      <c r="Z5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="3"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="17"/>
+      <c r="AD5" s="15"/>
+      <c r="AE5" s="15"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="2">
         <v>1</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="7">
+      <c r="D6" s="3"/>
+      <c r="E6" s="2">
         <v>3</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="2">
         <v>4</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="2">
         <v>5</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="2">
         <v>6</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="2">
         <v>7</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="2">
         <v>8</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="2">
         <v>9</v>
       </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7">
+      <c r="L6" s="2"/>
+      <c r="M6" s="2">
         <v>11</v>
       </c>
-      <c r="N6" s="7">
+      <c r="N6" s="2">
         <v>12</v>
       </c>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7">
+      <c r="O6" s="2"/>
+      <c r="P6" s="2">
         <v>14</v>
       </c>
-      <c r="Q6" s="7">
+      <c r="Q6" s="2">
         <v>15</v>
       </c>
-      <c r="R6" s="7">
+      <c r="R6" s="2">
         <v>16</v>
       </c>
-      <c r="S6" s="7">
+      <c r="S6" s="2">
+        <v>17</v>
+      </c>
+      <c r="T6" s="2">
+        <v>18</v>
+      </c>
+      <c r="U6" s="2">
         <v>19</v>
       </c>
-      <c r="T6" s="7">
+      <c r="V6" s="2">
         <v>20</v>
       </c>
-      <c r="U6" s="7">
+      <c r="W6" s="2">
         <v>21</v>
       </c>
-      <c r="V6" s="7">
+      <c r="X6" s="2">
         <v>22</v>
       </c>
-      <c r="W6" s="7">
+      <c r="Y6" s="2">
         <v>23</v>
       </c>
-      <c r="X6" s="7">
+      <c r="Z6" s="2">
         <v>25</v>
       </c>
-      <c r="Y6" s="7">
+      <c r="AA6" s="2">
         <v>24</v>
       </c>
-      <c r="Z6" s="7">
+      <c r="AB6" s="2">
         <v>26</v>
       </c>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="7">
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2">
         <v>27</v>
       </c>
-      <c r="AC6" s="7"/>
+      <c r="AE6" s="2"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A7" s="9">
-        <v>103</v>
-      </c>
-      <c r="B7" s="9" t="s">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>56010000371717</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="5">
         <v>6.2</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="6">
         <v>9238000</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="6">
         <v>1639000</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="10">
+      <c r="G7" s="5"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="5">
         <v>21</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="6">
         <v>2284170</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="5">
         <v>25</v>
       </c>
-      <c r="L7" s="11">
+      <c r="L7" s="6">
         <v>2719250</v>
       </c>
-      <c r="M7" s="10"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="10">
+      <c r="M7" s="5"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="5">
         <v>0.4</v>
       </c>
-      <c r="P7" s="11">
+      <c r="P7" s="6">
         <v>596000</v>
       </c>
-      <c r="Q7" s="10">
+      <c r="Q7" s="5">
         <v>1</v>
       </c>
-      <c r="R7" s="11">
+      <c r="R7" s="6">
         <v>2190000</v>
       </c>
-      <c r="S7" s="11">
+      <c r="S7" s="5">
+        <v>9.75</v>
+      </c>
+      <c r="T7" s="6">
+        <v>4875000</v>
+      </c>
+      <c r="U7" s="6">
         <v>23541420</v>
       </c>
-      <c r="T7" s="11">
+      <c r="V7" s="6">
         <v>1052894</v>
       </c>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11">
+      <c r="W7" s="6"/>
+      <c r="X7" s="6">
         <v>197418</v>
       </c>
-      <c r="W7" s="11">
+      <c r="Y7" s="6">
         <v>131612</v>
       </c>
-      <c r="X7" s="11">
+      <c r="Z7" s="6">
         <v>1381924</v>
       </c>
-      <c r="Y7" s="11">
+      <c r="AA7" s="6">
         <v>12947057</v>
       </c>
-      <c r="Z7" s="11">
+      <c r="AB7" s="6">
         <v>1779107</v>
       </c>
-      <c r="AA7" s="12"/>
-      <c r="AB7" s="11">
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="6">
         <v>7433332</v>
       </c>
-      <c r="AC7" s="13">
-        <v>56010001008221</v>
+      <c r="AE7" s="8">
+        <v>56010000371717</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A8" s="14">
-        <v>200</v>
-      </c>
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A8" s="13">
+        <v>56110000788758</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="10">
         <v>7.64</v>
       </c>
-      <c r="D8" s="16">
+      <c r="D8" s="11">
         <v>11383600</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="10">
         <v>1</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="11">
         <v>1490000</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="15">
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="10">
         <v>33</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="11">
         <v>4248288</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8" s="10">
         <v>25</v>
       </c>
-      <c r="L8" s="16">
+      <c r="L8" s="11">
         <v>3218400</v>
       </c>
-      <c r="M8" s="15"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="15">
+      <c r="M8" s="10"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="10">
         <v>0.4</v>
       </c>
-      <c r="P8" s="16">
+      <c r="P8" s="11">
         <v>596000</v>
       </c>
-      <c r="Q8" s="15">
+      <c r="Q8" s="10">
         <v>1</v>
       </c>
-      <c r="R8" s="16">
+      <c r="R8" s="11">
         <v>2592000</v>
       </c>
-      <c r="S8" s="16">
+      <c r="S8" s="5">
+        <v>7.1</v>
+      </c>
+      <c r="T8" s="6">
+        <v>4150000</v>
+      </c>
+      <c r="U8" s="11">
         <v>27678288</v>
       </c>
-      <c r="T8" s="16">
+      <c r="V8" s="11">
         <v>1369751</v>
       </c>
-      <c r="U8" s="16"/>
-      <c r="V8" s="16">
+      <c r="W8" s="11"/>
+      <c r="X8" s="11">
         <v>256828</v>
       </c>
-      <c r="W8" s="16">
+      <c r="Y8" s="11">
         <v>171219</v>
       </c>
-      <c r="X8" s="16">
+      <c r="Z8" s="11">
         <v>1797798</v>
       </c>
-      <c r="Y8" s="16">
+      <c r="AA8" s="11">
         <v>2615800</v>
       </c>
-      <c r="Z8" s="16">
+      <c r="AB8" s="11">
         <v>5463378</v>
       </c>
-      <c r="AA8" s="17"/>
-      <c r="AB8" s="16">
+      <c r="AC8" s="12"/>
+      <c r="AD8" s="11">
         <v>17801312</v>
       </c>
-      <c r="AC8" s="18">
-        <v>56010000080730</v>
+      <c r="AE8" s="13">
+        <v>56110000788758</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>56110000260797</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5">
+        <v>6.2</v>
+      </c>
+      <c r="D9" s="6">
+        <v>9238000</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1639000</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="5">
+        <v>21</v>
+      </c>
+      <c r="J9" s="6">
+        <v>2284170</v>
+      </c>
+      <c r="K9" s="5">
+        <v>25</v>
+      </c>
+      <c r="L9" s="6">
+        <v>2719250</v>
+      </c>
+      <c r="M9" s="5"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="P9" s="6">
+        <v>596000</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>1</v>
+      </c>
+      <c r="R9" s="6">
+        <v>2190000</v>
+      </c>
+      <c r="S9" s="5">
+        <v>7.1</v>
+      </c>
+      <c r="T9" s="6">
+        <v>3550000</v>
+      </c>
+      <c r="U9" s="6">
+        <v>23541420</v>
+      </c>
+      <c r="V9" s="6">
+        <v>1052894</v>
+      </c>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6">
+        <v>197418</v>
+      </c>
+      <c r="Y9" s="6">
+        <v>131612</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>1381924</v>
+      </c>
+      <c r="AA9" s="6">
+        <v>12947057</v>
+      </c>
+      <c r="AB9" s="6">
+        <v>1779107</v>
+      </c>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="6">
+        <v>7433332</v>
+      </c>
+      <c r="AE9" s="8">
+        <v>56110000260797</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A10" s="13">
+        <v>56110000260414</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="10">
+        <v>7.64</v>
+      </c>
+      <c r="D10" s="11">
+        <v>11383600</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="11">
+        <v>1490000</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="10">
+        <v>33</v>
+      </c>
+      <c r="J10" s="11">
+        <v>4248288</v>
+      </c>
+      <c r="K10" s="10">
+        <v>25</v>
+      </c>
+      <c r="L10" s="11">
+        <v>3218400</v>
+      </c>
+      <c r="M10" s="10"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="P10" s="11">
+        <v>596000</v>
+      </c>
+      <c r="Q10" s="10">
+        <v>1</v>
+      </c>
+      <c r="R10" s="11">
+        <v>2592000</v>
+      </c>
+      <c r="S10" s="10">
+        <v>7.1</v>
+      </c>
+      <c r="T10" s="11">
+        <v>3550000</v>
+      </c>
+      <c r="U10" s="11">
+        <v>27678288</v>
+      </c>
+      <c r="V10" s="11">
+        <v>1369751</v>
+      </c>
+      <c r="W10" s="11"/>
+      <c r="X10" s="11">
+        <v>256828</v>
+      </c>
+      <c r="Y10" s="11">
+        <v>171219</v>
+      </c>
+      <c r="Z10" s="11">
+        <v>1797798</v>
+      </c>
+      <c r="AA10" s="11">
+        <v>2615800</v>
+      </c>
+      <c r="AB10" s="11">
+        <v>5463378</v>
+      </c>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="11">
+        <v>17801312</v>
+      </c>
+      <c r="AE10" s="13">
+        <v>56110000260414</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="AB4:AB5"/>
-    <mergeCell ref="AC4:AC5"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="T4:X4"/>
-    <mergeCell ref="Y4:Y5"/>
-    <mergeCell ref="Z4:Z5"/>
-    <mergeCell ref="AA4:AA5"/>
+  <mergeCells count="19">
     <mergeCell ref="I2:W2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
@@ -1103,6 +1307,15 @@
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="AD4:AD5"/>
+    <mergeCell ref="AE4:AE5"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="V4:Z4"/>
+    <mergeCell ref="AA4:AA5"/>
+    <mergeCell ref="AB4:AB5"/>
+    <mergeCell ref="AC4:AC5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>